<commit_message>
modify ch6 xlsx , ch7 xlsx
</commit_message>
<xml_diff>
--- a/doc/ch6/工作項目與時程.xlsx
+++ b/doc/ch6/工作項目與時程.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>任務名稱</t>
   </si>
@@ -75,9 +75,6 @@
     <t>系統架構</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>編程標準</t>
   </si>
   <si>
@@ -100,12 +97,6 @@
   </si>
   <si>
     <t>個人資訊編輯</t>
-  </si>
-  <si>
-    <t>個人社群網路建置</t>
-  </si>
-  <si>
-    <t>頭像編輯</t>
   </si>
   <si>
     <t>系統測試</t>
@@ -131,6 +122,14 @@
       </rPr>
       <t>建置</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>全體</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>實作小組</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -698,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV61"/>
+  <dimension ref="A1:IV59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -947,17 +946,17 @@
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7">
+        <v>40109</v>
+      </c>
+      <c r="F12" s="7">
+        <v>40109</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -968,19 +967,19 @@
     <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7">
+        <v>40110</v>
+      </c>
+      <c r="F13" s="7">
+        <v>40110</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -991,19 +990,19 @@
     <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="7">
+        <v>40110</v>
+      </c>
+      <c r="F14" s="7">
+        <v>40110</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1013,7 +1012,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1029,13 +1028,13 @@
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="7">
         <v>40110</v>
@@ -1052,13 +1051,13 @@
     <row r="17" spans="1:11" ht="15.75">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="7">
         <v>40110</v>
@@ -1075,13 +1074,13 @@
     <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="7">
         <v>40111</v>
@@ -1098,13 +1097,13 @@
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E19" s="7">
         <v>40111</v>
@@ -1121,13 +1120,13 @@
     <row r="20" spans="1:11" ht="15.75">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E20" s="7">
         <v>40112</v>
@@ -1142,22 +1141,14 @@
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="15.75">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1167,19 +1158,19 @@
     <row r="22" spans="1:11" ht="15.75">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="E22" s="7">
+        <v>40113</v>
+      </c>
+      <c r="F22" s="7">
+        <v>40115</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1188,14 +1179,12 @@
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="15.75">
-      <c r="A23" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1204,21 +1193,11 @@
     </row>
     <row r="24" spans="1:11" ht="15.75">
       <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="7">
-        <v>40115</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1680,32 +1659,6 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-    </row>
-    <row r="61" spans="1:11" ht="15.75">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.78740149736404419" right="0.78740149736404419" top="0.78740149736404419" bottom="0.78740149736404419" header="0.39370083808898926" footer="0.39370083808898926"/>

</xml_diff>